<commit_message>
read dtc info report by status mask implemented
</commit_message>
<xml_diff>
--- a/logic/uds_py/uds.xlsx
+++ b/logic/uds_py/uds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\qt\uds_sniffer\logic\uds_py\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\qt\uds_tracer\logic\uds_py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1577A4D-BD98-4009-AC4F-A27929030183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFF1CAB-C6D4-4243-AB13-CED0EA766D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14805" activeTab="2" xr2:uid="{78E47929-975A-436B-84A5-DC2091DE310C}"/>
+    <workbookView xWindow="4800" yWindow="810" windowWidth="21600" windowHeight="10605" activeTab="2" xr2:uid="{78E47929-975A-436B-84A5-DC2091DE310C}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="737">
   <si>
     <t>posResp</t>
   </si>
@@ -2228,6 +2228,51 @@
   </si>
   <si>
     <t>paramRecord</t>
+  </si>
+  <si>
+    <t>mask</t>
+  </si>
+  <si>
+    <t>reportType</t>
+  </si>
+  <si>
+    <t>availStMask</t>
+  </si>
+  <si>
+    <t>dtcNStRecord</t>
+  </si>
+  <si>
+    <t>ReadDTCInfoBySt</t>
+  </si>
+  <si>
+    <t>ReadDTCInfoByStPos</t>
+  </si>
+  <si>
+    <t>ReadDtcInfoGeneric</t>
+  </si>
+  <si>
+    <t>buf</t>
+  </si>
+  <si>
+    <t>dtcHighByte</t>
+  </si>
+  <si>
+    <t>DtcNStatusRecordPos</t>
+  </si>
+  <si>
+    <t>dtcMiddleByte</t>
+  </si>
+  <si>
+    <t>dtcLowByte</t>
+  </si>
+  <si>
+    <t>statusOfDtc</t>
+  </si>
+  <si>
+    <t>ReadDTCInfoByStPos dtcNStRecord content</t>
+  </si>
+  <si>
+    <t>ReadDtcInfoGenericPos</t>
   </si>
 </sst>
 </file>
@@ -2683,8 +2728,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}" name="Table8" displayName="Table8" ref="A1:F59" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:F59" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}" name="Table8" displayName="Table8" ref="A1:F76" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:F76" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7050B423-F41F-4BBD-A218-F58815E56653}" uniqueName="MemClassName" name="MemClassName">
       <xmlColumnPr mapId="17" xpath="/ReqResp/ReqRespItem/MemClassName" xmlDataType="string"/>
@@ -3022,7 +3067,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3611,8 +3656,8 @@
   <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7167,25 +7212,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4B2C54-A138-47B8-96DC-B258FA5CCF76}">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63:C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="192.85546875" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>685</v>
       </c>
@@ -7204,11 +7249,11 @@
       <c r="F1" t="s">
         <v>637</v>
       </c>
-      <c r="N1" t="s">
+      <c r="M1" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>689</v>
       </c>
@@ -7225,7 +7270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>689</v>
       </c>
@@ -7242,7 +7287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>689</v>
       </c>
@@ -7259,7 +7304,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>638</v>
       </c>
@@ -7276,11 +7321,11 @@
         <v>1</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="N5" t="s">
+      <c r="M5" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>638</v>
       </c>
@@ -7297,11 +7342,11 @@
         <v>1</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="N6" t="s">
+      <c r="M6" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>638</v>
       </c>
@@ -7319,7 +7364,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>639</v>
       </c>
@@ -7337,7 +7382,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>639</v>
       </c>
@@ -7355,7 +7400,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>639</v>
       </c>
@@ -7373,7 +7418,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>644</v>
       </c>
@@ -7391,7 +7436,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>644</v>
       </c>
@@ -7411,7 +7456,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>644</v>
       </c>
@@ -7429,7 +7474,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>643</v>
       </c>
@@ -7447,7 +7492,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>643</v>
       </c>
@@ -7467,7 +7512,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>646</v>
       </c>
@@ -8278,10 +8323,302 @@
         <v>631</v>
       </c>
     </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>728</v>
+      </c>
+      <c r="B60" t="s">
+        <v>630</v>
+      </c>
+      <c r="C60" t="s">
+        <v>488</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>728</v>
+      </c>
+      <c r="B61" t="s">
+        <v>640</v>
+      </c>
+      <c r="C61" t="s">
+        <v>488</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>728</v>
+      </c>
+      <c r="B62" t="s">
+        <v>729</v>
+      </c>
+      <c r="C62" t="s">
+        <v>488</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>736</v>
+      </c>
+      <c r="B63" t="s">
+        <v>630</v>
+      </c>
+      <c r="C63" t="s">
+        <v>487</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>736</v>
+      </c>
+      <c r="B64" t="s">
+        <v>640</v>
+      </c>
+      <c r="C64" t="s">
+        <v>487</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>736</v>
+      </c>
+      <c r="B65" t="s">
+        <v>729</v>
+      </c>
+      <c r="C65" t="s">
+        <v>487</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B66" t="s">
+        <v>630</v>
+      </c>
+      <c r="C66" t="s">
+        <v>488</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B67" t="s">
+        <v>640</v>
+      </c>
+      <c r="C67" t="s">
+        <v>488</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B68" t="s">
+        <v>722</v>
+      </c>
+      <c r="C68" t="s">
+        <v>488</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="B69" t="s">
+        <v>630</v>
+      </c>
+      <c r="C69" t="s">
+        <v>487</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="B70" t="s">
+        <v>723</v>
+      </c>
+      <c r="C70" t="s">
+        <v>487</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="B71" t="s">
+        <v>724</v>
+      </c>
+      <c r="C71" t="s">
+        <v>487</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="B72" t="s">
+        <v>725</v>
+      </c>
+      <c r="C72" t="s">
+        <v>487</v>
+      </c>
+      <c r="D72">
+        <v>4</v>
+      </c>
+      <c r="E72" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>731</v>
+      </c>
+      <c r="B73" t="s">
+        <v>730</v>
+      </c>
+      <c r="C73" t="s">
+        <v>487</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>731</v>
+      </c>
+      <c r="B74" t="s">
+        <v>732</v>
+      </c>
+      <c r="C74" t="s">
+        <v>487</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>731</v>
+      </c>
+      <c r="B75" t="s">
+        <v>733</v>
+      </c>
+      <c r="C75" t="s">
+        <v>487</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>731</v>
+      </c>
+      <c r="B76" t="s">
+        <v>734</v>
+      </c>
+      <c r="C76" t="s">
+        <v>487</v>
+      </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C1048576 C1:C7" xr:uid="{D2E22386-73BA-4047-9AD9-9DD498405CB6}">
-      <formula1>$N$5:$N$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C7 C9:C1048576" xr:uid="{D2E22386-73BA-4047-9AD9-9DD498405CB6}">
+      <formula1>$M$5:$M$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
diag p2 server added c template fix
</commit_message>
<xml_diff>
--- a/logic/uds_py/uds.xlsx
+++ b/logic/uds_py/uds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\qt\uds_tracer\logic\uds_py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFF1CAB-C6D4-4243-AB13-CED0EA766D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16A04F-6FB7-4787-B0B9-A09047190AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="810" windowWidth="21600" windowHeight="10605" activeTab="2" xr2:uid="{78E47929-975A-436B-84A5-DC2091DE310C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14805" activeTab="2" xr2:uid="{78E47929-975A-436B-84A5-DC2091DE310C}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="737">
   <si>
     <t>posResp</t>
   </si>
@@ -1988,13 +1988,7 @@
     <t>DiagSessCtrlPos</t>
   </si>
   <si>
-    <t>sessParam</t>
-  </si>
-  <si>
     <t>diagnosticSessionType. This parameter is an echo of bits 6 to 0 of the SubFunction parameter from the request message.</t>
-  </si>
-  <si>
-    <t>sessionParameterRecord. This parameter record contains session specific parameter values reported by the server. The content of the sessionParameterRecord is defined in Table 28 and Table 29.</t>
   </si>
   <si>
     <t>xx</t>
@@ -2230,9 +2224,15 @@
     <t>paramRecord</t>
   </si>
   <si>
+    <t>ReadDtcInfoBySt</t>
+  </si>
+  <si>
     <t>mask</t>
   </si>
   <si>
+    <t>ReadDtcInfoByStPos</t>
+  </si>
+  <si>
     <t>reportType</t>
   </si>
   <si>
@@ -2242,12 +2242,6 @@
     <t>dtcNStRecord</t>
   </si>
   <si>
-    <t>ReadDTCInfoBySt</t>
-  </si>
-  <si>
-    <t>ReadDTCInfoByStPos</t>
-  </si>
-  <si>
     <t>ReadDtcInfoGeneric</t>
   </si>
   <si>
@@ -2273,6 +2267,12 @@
   </si>
   <si>
     <t>ReadDtcInfoGenericPos</t>
+  </si>
+  <si>
+    <t>p2Server</t>
+  </si>
+  <si>
+    <t>p2StarServer</t>
   </si>
 </sst>
 </file>
@@ -2728,8 +2728,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}" name="Table8" displayName="Table8" ref="A1:F76" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:F76" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}" name="Table8" displayName="Table8" ref="A1:F77" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:F77" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7050B423-F41F-4BBD-A218-F58815E56653}" uniqueName="MemClassName" name="MemClassName">
       <xmlColumnPr mapId="17" xpath="/ReqResp/ReqRespItem/MemClassName" xmlDataType="string"/>
@@ -3125,7 +3125,7 @@
         <v>243</v>
       </c>
       <c r="F2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>253</v>
@@ -3151,7 +3151,7 @@
         <v>243</v>
       </c>
       <c r="F3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>256</v>
@@ -3177,7 +3177,7 @@
         <v>243</v>
       </c>
       <c r="F4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>258</v>
@@ -3226,7 +3226,7 @@
         <v>243</v>
       </c>
       <c r="F6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>269</v>
@@ -3349,7 +3349,7 @@
         <v>243</v>
       </c>
       <c r="F12" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3437,7 +3437,7 @@
         <v>243</v>
       </c>
       <c r="F17" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
         <v>243</v>
       </c>
       <c r="F18" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3528,7 +3528,7 @@
         <v>243</v>
       </c>
       <c r="F22" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3656,7 +3656,7 @@
   <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
@@ -6965,22 +6965,22 @@
         <v>410</v>
       </c>
       <c r="B144" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C144" t="s">
         <v>311</v>
       </c>
       <c r="D144" t="s">
+        <v>688</v>
+      </c>
+      <c r="E144" t="s">
+        <v>377</v>
+      </c>
+      <c r="F144" t="s">
+        <v>689</v>
+      </c>
+      <c r="G144" t="s">
         <v>690</v>
-      </c>
-      <c r="E144" t="s">
-        <v>377</v>
-      </c>
-      <c r="F144" t="s">
-        <v>691</v>
-      </c>
-      <c r="G144" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -6988,22 +6988,22 @@
         <v>410</v>
       </c>
       <c r="B145" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C145" t="s">
         <v>379</v>
       </c>
       <c r="D145" t="s">
+        <v>691</v>
+      </c>
+      <c r="E145" t="s">
+        <v>377</v>
+      </c>
+      <c r="F145" t="s">
+        <v>692</v>
+      </c>
+      <c r="G145" t="s">
         <v>693</v>
-      </c>
-      <c r="E145" t="s">
-        <v>377</v>
-      </c>
-      <c r="F145" t="s">
-        <v>694</v>
-      </c>
-      <c r="G145" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -7011,22 +7011,22 @@
         <v>410</v>
       </c>
       <c r="B146" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C146" t="s">
         <v>380</v>
       </c>
       <c r="D146" t="s">
+        <v>694</v>
+      </c>
+      <c r="E146" t="s">
+        <v>377</v>
+      </c>
+      <c r="F146" t="s">
+        <v>695</v>
+      </c>
+      <c r="G146" t="s">
         <v>696</v>
-      </c>
-      <c r="E146" t="s">
-        <v>377</v>
-      </c>
-      <c r="F146" t="s">
-        <v>697</v>
-      </c>
-      <c r="G146" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -7034,22 +7034,22 @@
         <v>410</v>
       </c>
       <c r="B147" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C147" t="s">
         <v>394</v>
       </c>
       <c r="D147" t="s">
+        <v>697</v>
+      </c>
+      <c r="E147" t="s">
+        <v>377</v>
+      </c>
+      <c r="F147" t="s">
+        <v>698</v>
+      </c>
+      <c r="G147" t="s">
         <v>699</v>
-      </c>
-      <c r="E147" t="s">
-        <v>377</v>
-      </c>
-      <c r="F147" t="s">
-        <v>700</v>
-      </c>
-      <c r="G147" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -7057,22 +7057,22 @@
         <v>410</v>
       </c>
       <c r="B148" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C148" t="s">
         <v>396</v>
       </c>
       <c r="D148" t="s">
+        <v>700</v>
+      </c>
+      <c r="E148" t="s">
+        <v>377</v>
+      </c>
+      <c r="F148" t="s">
+        <v>701</v>
+      </c>
+      <c r="G148" t="s">
         <v>702</v>
-      </c>
-      <c r="E148" t="s">
-        <v>377</v>
-      </c>
-      <c r="F148" t="s">
-        <v>703</v>
-      </c>
-      <c r="G148" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -7080,22 +7080,22 @@
         <v>410</v>
       </c>
       <c r="B149" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C149" t="s">
         <v>457</v>
       </c>
       <c r="D149" t="s">
+        <v>703</v>
+      </c>
+      <c r="E149" t="s">
+        <v>377</v>
+      </c>
+      <c r="F149" t="s">
+        <v>704</v>
+      </c>
+      <c r="G149" t="s">
         <v>705</v>
-      </c>
-      <c r="E149" t="s">
-        <v>377</v>
-      </c>
-      <c r="F149" t="s">
-        <v>706</v>
-      </c>
-      <c r="G149" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -7126,7 +7126,7 @@
         <v>410</v>
       </c>
       <c r="B151" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C151" t="s">
         <v>399</v>
@@ -7212,11 +7212,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4B2C54-A138-47B8-96DC-B258FA5CCF76}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63:C65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7232,7 +7232,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B1" t="s">
         <v>237</v>
@@ -7255,7 +7255,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>630</v>
@@ -7272,7 +7272,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>640</v>
@@ -7289,10 +7289,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>488</v>
@@ -7547,59 +7547,55 @@
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>647</v>
+      <c r="B18" t="s">
+        <v>735</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>3</v>
       </c>
-      <c r="E18" s="3">
-        <v>4</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>649</v>
+      <c r="E18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>630</v>
+        <v>646</v>
+      </c>
+      <c r="B19" t="s">
+        <v>736</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>487</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -7608,16 +7604,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -7626,322 +7622,322 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>654</v>
+        <v>640</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D23" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>248</v>
+        <v>650</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D24" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F24" s="10" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>657</v>
+        <v>248</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F26" s="10" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
       </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F28" s="10" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>660</v>
+        <v>630</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="D30" s="3">
         <v>2</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="F30" s="10" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>630</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>663</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="D32" s="3">
         <v>2</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>630</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="10" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>660</v>
+        <v>630</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="3">
-        <v>2</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>667</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D34" s="3">
-        <v>4</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>631</v>
+        <v>2</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>630</v>
+        <v>664</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D35" s="3">
-        <v>1</v>
-      </c>
-      <c r="E35" s="3">
-        <v>1</v>
-      </c>
-      <c r="F35" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>660</v>
+        <v>630</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D36" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="3">
-        <v>2</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>670</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>630</v>
+        <v>658</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="3">
-        <v>1</v>
-      </c>
-      <c r="F37" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -7950,168 +7946,168 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>673</v>
+        <v>640</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D39" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>488</v>
       </c>
       <c r="D40" s="3">
-        <v>5</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>631</v>
+        <v>3</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2</v>
       </c>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>630</v>
+        <v>672</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>631</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>676</v>
+        <v>630</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D42" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="3">
         <v>1</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>679</v>
-      </c>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D43" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D44" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>675</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>678</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D45" s="3">
-        <v>6</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>683</v>
+        <v>673</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>630</v>
+        <v>676</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>487</v>
       </c>
       <c r="D46" s="3">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3">
-        <v>1</v>
-      </c>
-      <c r="F46" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>686</v>
+        <v>630</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>687</v>
+      <c r="D47" s="3">
+        <v>1</v>
       </c>
       <c r="E47" s="3">
         <v>1</v>
@@ -8120,7 +8116,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>684</v>
@@ -8129,280 +8125,281 @@
         <v>487</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="E48" s="3">
         <v>1</v>
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>715</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>713</v>
+      </c>
+      <c r="B50" t="s">
         <v>630</v>
-      </c>
-      <c r="C49" t="s">
-        <v>488</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>715</v>
-      </c>
-      <c r="B50" t="s">
-        <v>640</v>
       </c>
       <c r="C50" t="s">
         <v>488</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B51" t="s">
-        <v>716</v>
+        <v>640</v>
       </c>
       <c r="C51" t="s">
         <v>488</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B52" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="C52" t="s">
         <v>488</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>713</v>
+      </c>
+      <c r="B53" t="s">
         <v>715</v>
-      </c>
-      <c r="B53" t="s">
-        <v>718</v>
       </c>
       <c r="C53" t="s">
         <v>488</v>
       </c>
       <c r="D53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>272</v>
+        <v>713</v>
       </c>
       <c r="B54" t="s">
-        <v>630</v>
+        <v>716</v>
       </c>
       <c r="C54" t="s">
         <v>488</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>272</v>
       </c>
       <c r="B55" t="s">
-        <v>719</v>
+        <v>630</v>
       </c>
       <c r="C55" t="s">
         <v>488</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>272</v>
       </c>
       <c r="B56" t="s">
-        <v>663</v>
+        <v>717</v>
       </c>
       <c r="C56" t="s">
         <v>488</v>
       </c>
       <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>272</v>
+      </c>
+      <c r="B57" t="s">
+        <v>661</v>
+      </c>
+      <c r="C57" t="s">
+        <v>488</v>
+      </c>
+      <c r="D57">
         <v>3</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>720</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>718</v>
+      </c>
+      <c r="B58" t="s">
         <v>630</v>
-      </c>
-      <c r="C57" t="s">
-        <v>487</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>720</v>
-      </c>
-      <c r="B58" t="s">
-        <v>719</v>
       </c>
       <c r="C58" t="s">
         <v>487</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B59" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C59" t="s">
         <v>487</v>
       </c>
       <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>718</v>
+      </c>
+      <c r="B60" t="s">
+        <v>719</v>
+      </c>
+      <c r="C60" t="s">
+        <v>487</v>
+      </c>
+      <c r="D60">
         <v>3</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>728</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>726</v>
+      </c>
+      <c r="B61" t="s">
         <v>630</v>
-      </c>
-      <c r="C60" t="s">
-        <v>488</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>728</v>
-      </c>
-      <c r="B61" t="s">
-        <v>640</v>
       </c>
       <c r="C61" t="s">
         <v>488</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B62" t="s">
-        <v>729</v>
+        <v>640</v>
       </c>
       <c r="C62" t="s">
         <v>488</v>
       </c>
       <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>726</v>
+      </c>
+      <c r="B63" t="s">
+        <v>727</v>
+      </c>
+      <c r="C63" t="s">
+        <v>488</v>
+      </c>
+      <c r="D63">
         <v>3</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>736</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>734</v>
+      </c>
+      <c r="B64" t="s">
         <v>630</v>
-      </c>
-      <c r="C63" t="s">
-        <v>487</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>736</v>
-      </c>
-      <c r="B64" t="s">
-        <v>640</v>
       </c>
       <c r="C64" t="s">
         <v>487</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -8410,50 +8407,50 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B65" t="s">
-        <v>729</v>
+        <v>640</v>
       </c>
       <c r="C65" t="s">
         <v>487</v>
       </c>
       <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>734</v>
+      </c>
+      <c r="B66" t="s">
+        <v>727</v>
+      </c>
+      <c r="C66" t="s">
+        <v>487</v>
+      </c>
+      <c r="D66">
         <v>3</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>631</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>726</v>
-      </c>
-      <c r="B66" t="s">
-        <v>630</v>
-      </c>
-      <c r="C66" t="s">
-        <v>488</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B67" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C67" t="s">
         <v>488</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -8461,16 +8458,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B68" t="s">
-        <v>722</v>
+        <v>640</v>
       </c>
       <c r="C68" t="s">
         <v>488</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -8478,16 +8475,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="B69" t="s">
-        <v>630</v>
+        <v>721</v>
       </c>
       <c r="C69" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -8495,16 +8492,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="B70" t="s">
-        <v>723</v>
+        <v>630</v>
       </c>
       <c r="C70" t="s">
         <v>487</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -8512,16 +8509,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="B71" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C71" t="s">
         <v>487</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -8529,70 +8526,70 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="B72" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C72" t="s">
         <v>487</v>
       </c>
       <c r="D72">
-        <v>4</v>
-      </c>
-      <c r="E72" t="s">
-        <v>631</v>
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>731</v>
+      <c r="A73" s="5" t="s">
+        <v>722</v>
       </c>
       <c r="B73" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="C73" t="s">
         <v>487</v>
       </c>
       <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>735</v>
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B74" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="C74" t="s">
         <v>487</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
+      <c r="F74" s="5" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B75" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C75" t="s">
         <v>487</v>
       </c>
       <c r="D75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -8600,18 +8597,35 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>729</v>
+      </c>
+      <c r="B76" t="s">
         <v>731</v>
-      </c>
-      <c r="B76" t="s">
-        <v>734</v>
       </c>
       <c r="C76" t="s">
         <v>487</v>
       </c>
       <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>729</v>
+      </c>
+      <c r="B77" t="s">
+        <v>732</v>
+      </c>
+      <c r="C77" t="s">
+        <v>487</v>
+      </c>
+      <c r="D77">
         <v>4</v>
       </c>
-      <c r="E76">
+      <c r="E77">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clear dtc info implemented
</commit_message>
<xml_diff>
--- a/logic/uds_py/uds.xlsx
+++ b/logic/uds_py/uds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\qt\uds_tracer\logic\uds_py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16A04F-6FB7-4787-B0B9-A09047190AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5261516-E2F4-4A9B-AD1B-91B3E7CBAA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14805" activeTab="2" xr2:uid="{78E47929-975A-436B-84A5-DC2091DE310C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="740">
   <si>
     <t>posResp</t>
   </si>
@@ -2273,6 +2273,15 @@
   </si>
   <si>
     <t>p2StarServer</t>
+  </si>
+  <si>
+    <t>ClearDtcInfo</t>
+  </si>
+  <si>
+    <t>memorySelection</t>
+  </si>
+  <si>
+    <t>ClearDtcInfoResp</t>
   </si>
 </sst>
 </file>
@@ -2728,8 +2737,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}" name="Table8" displayName="Table8" ref="A1:F77" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:F77" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}" name="Table8" displayName="Table8" ref="A1:F83" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:F83" xr:uid="{BC95CCAA-C22D-43DE-929A-961CEDE5CDBA}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7050B423-F41F-4BBD-A218-F58815E56653}" uniqueName="MemClassName" name="MemClassName">
       <xmlColumnPr mapId="17" xpath="/ReqResp/ReqRespItem/MemClassName" xmlDataType="string"/>
@@ -7212,11 +7221,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4B2C54-A138-47B8-96DC-B258FA5CCF76}">
-  <dimension ref="A1:M77"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8626,6 +8635,108 @@
         <v>4</v>
       </c>
       <c r="E77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>737</v>
+      </c>
+      <c r="B78" t="s">
+        <v>630</v>
+      </c>
+      <c r="C78" t="s">
+        <v>488</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>737</v>
+      </c>
+      <c r="B79" t="s">
+        <v>728</v>
+      </c>
+      <c r="C79" t="s">
+        <v>488</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>737</v>
+      </c>
+      <c r="B80" t="s">
+        <v>730</v>
+      </c>
+      <c r="C80" t="s">
+        <v>488</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>737</v>
+      </c>
+      <c r="B81" t="s">
+        <v>731</v>
+      </c>
+      <c r="C81" t="s">
+        <v>488</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>737</v>
+      </c>
+      <c r="B82" t="s">
+        <v>738</v>
+      </c>
+      <c r="C82" t="s">
+        <v>488</v>
+      </c>
+      <c r="D82">
+        <v>5</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>739</v>
+      </c>
+      <c r="B83" t="s">
+        <v>630</v>
+      </c>
+      <c r="C83" t="s">
+        <v>487</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
         <v>1</v>
       </c>
     </row>

</xml_diff>